<commit_message>
More PCB tidying up
</commit_message>
<xml_diff>
--- a/mini/mini_rev1/aqp_mini_rev1_BOM.xlsx
+++ b/mini/mini_rev1/aqp_mini_rev1_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\System\pcb\mini\mini_rev1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E69C42D-020D-4B37-B152-C5FC08D1E761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFDD070-F39C-4D89-8273-0FA6C0F61AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="1815" windowWidth="12360" windowHeight="11295" xr2:uid="{6215E24B-0129-4333-86D9-7A479FB72631}"/>
+    <workbookView xWindow="1425" yWindow="2400" windowWidth="12360" windowHeight="11295" xr2:uid="{6215E24B-0129-4333-86D9-7A479FB72631}"/>
   </bookViews>
   <sheets>
     <sheet name="aquarius-plus_bom" sheetId="2" r:id="rId1"/>
@@ -265,9 +265,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>L_CommonMode_Wurth_WE-CNSW-1206</t>
-  </si>
-  <si>
     <t>USB Choke</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
     <t>220 @ 100mHz</t>
   </si>
   <si>
-    <t>C2649327</t>
-  </si>
-  <si>
     <t>3.0mm Blue LED</t>
   </si>
   <si>
@@ -401,6 +395,12 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>L_CommonMode_Wurth_WE-CNSW-0805</t>
+  </si>
+  <si>
+    <t>C2649324</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1338,21 +1338,21 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1380,21 +1380,21 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1520,12 +1520,12 @@
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>34</v>
@@ -1534,7 +1534,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,12 +1688,12 @@
         <v>61</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>63</v>
@@ -1702,7 +1702,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1716,7 +1716,7 @@
         <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
         <v>75</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1772,35 +1772,35 @@
         <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>